<commit_message>
Scraping procedure for alternative page layouts, saving images and links
</commit_message>
<xml_diff>
--- a/productpages.xlsx
+++ b/productpages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/morganoneka/Documents/PersonalProjects/haircare/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC4E353-54D0-0245-A371-320D0205A01C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75737365-CA66-1148-A9EC-AA5FDF360090}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{BCF382E2-ED57-B94B-B06D-7D1A2B33F2F8}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="79">
   <si>
     <t>Brand</t>
   </si>
@@ -217,6 +217,60 @@
   </si>
   <si>
     <t>https://www.amazon.com/stores/page/3E2D6F31-1B01-4500-816F-26E1D001AF7B?ingress=2&amp;visitId=f4c98e26-d71e-4a2c-8f85-46c44d9229da&amp;ref_=ast_bln</t>
+  </si>
+  <si>
+    <t>Curl Talk</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/stores/page/1DB8A150-0F33-43F4-B681-6911B16BF1BD?ingress=2&amp;visitId=3dec1212-38b5-45f5-b1df-26f94b3a7df5&amp;ref_=ast_bln</t>
+  </si>
+  <si>
+    <t>As I Am</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/s?k=As+I+Am&amp;rh=n%3A3760911%2Cp_89%3AAs+I+Am&amp;dc&amp;qid=1650565270&amp;rnid=2528832011&amp;ref=sr_nr_p_89_1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/s?k=As+I+Am&amp;i=beauty&amp;rh=n%3A3760911%2Cp_89%3AAs+I+Am&amp;dc&amp;page=2&amp;qid=1650565503&amp;rnid=2528832011&amp;ref=sr_pg_2</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/s?k=As+I+Am&amp;i=beauty&amp;rh=n%3A3760911%2Cp_89%3AAs+I+Am&amp;dc&amp;page=3&amp;qid=1650566832&amp;rnid=2528832011&amp;ref=sr_pg_3</t>
+  </si>
+  <si>
+    <t>Jessicurl</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/s?k=jessicurl&amp;rh=n%3A3760911%2Cp_89%3AJessicurl&amp;dc&amp;crid=1IP2JU854JO9R&amp;qid=1650566942&amp;rnid=2528832011&amp;sprefix=jessicurl%2Caps%2C105&amp;ref=sr_nr_p_89_1</t>
+  </si>
+  <si>
+    <t>Kinky Curly</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/s?k=Kinky+Curly&amp;rh=n%3A3760911%2Cp_89%3AKinky+Curly&amp;dc&amp;qid=1650567033&amp;rnid=2528832011&amp;ref=sr_nr_p_89_1</t>
+  </si>
+  <si>
+    <t>Ouidad</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/s?k=ouidad+hair+products+for+curly+hair&amp;rh=n%3A3760911%2Cp_89%3AOuidad&amp;dc&amp;qid=1650567090&amp;rnid=2528832011&amp;sprefix=ouidad%2Caps%2C102&amp;ref=sr_nr_p_89_1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/s?k=ouidad+hair+products+for+curly+hair&amp;i=beauty&amp;rh=n%3A3760911%2Cp_89%3AOuidad&amp;dc&amp;page=2&amp;qid=1650567094&amp;rnid=2528832011&amp;sprefix=ouidad%2Caps%2C102&amp;ref=sr_pg_1</t>
+  </si>
+  <si>
+    <t>Dippity Do</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/s?k=Dippity+Do&amp;rh=n%3A3760911%2Cp_89%3ADippity+Do&amp;dc&amp;qid=1650567154&amp;rnid=2528832011&amp;ref=sr_nr_p_89_1</t>
+  </si>
+  <si>
+    <t>pg1</t>
+  </si>
+  <si>
+    <t>pg2</t>
+  </si>
+  <si>
+    <t>pg3</t>
   </si>
 </sst>
 </file>
@@ -579,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D25933B8-7191-7A43-9709-6FB6A19CFFAF}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -862,7 +916,109 @@
         <v>60</v>
       </c>
     </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" t="s">
+        <v>76</v>
+      </c>
+      <c r="C30" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" t="s">
+        <v>77</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" t="s">
+        <v>76</v>
+      </c>
+      <c r="C34" t="s">
+        <v>75</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C33" r:id="rId1" xr:uid="{840F3526-DAEC-3845-B161-1F83DAFA8171}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed filter issue for products with multiple type tags
</commit_message>
<xml_diff>
--- a/productpages.xlsx
+++ b/productpages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/morganoneka/Documents/PersonalProjects/haircare/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75737365-CA66-1148-A9EC-AA5FDF360090}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A8C133-EBF4-CA47-B834-7450BF74A2C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{BCF382E2-ED57-B94B-B06D-7D1A2B33F2F8}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="81">
   <si>
     <t>Brand</t>
   </si>
@@ -271,6 +271,12 @@
   </si>
   <si>
     <t>pg3</t>
+  </si>
+  <si>
+    <t>Aveda</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/s?k=Aveda&amp;rh=n%3A3760911%2Cp_89%3AAveda&amp;dc&amp;qid=1650933740&amp;rnid=2528832011&amp;ref=sr_nr_p_89_1</t>
   </si>
 </sst>
 </file>
@@ -633,10 +639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D25933B8-7191-7A43-9709-6FB6A19CFFAF}">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1015,6 +1021,17 @@
         <v>75</v>
       </c>
     </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>79</v>
+      </c>
+      <c r="B35" t="s">
+        <v>76</v>
+      </c>
+      <c r="C35" t="s">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C33" r:id="rId1" xr:uid="{840F3526-DAEC-3845-B161-1F83DAFA8171}"/>

</xml_diff>